<commit_message>
Test Decission Tree and SVM classifiers
</commit_message>
<xml_diff>
--- a/Version Testing.xlsx
+++ b/Version Testing.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Programming\Udacity\ud120-projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A401EE79-9DEC-447E-956E-D1888997DEE6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52830" yWindow="1920" windowWidth="22110" windowHeight="16455" activeTab="2" xr2:uid="{C7B2D404-27C9-4797-AF56-72570EB8FE56}"/>
+    <workbookView xWindow="52830" yWindow="1920" windowWidth="22110" windowHeight="16455" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Ver 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Ver 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Ver 3" sheetId="3" r:id="rId3"/>
+    <sheet name="NB Ver 1" sheetId="1" r:id="rId1"/>
+    <sheet name="NB Ver 2" sheetId="2" r:id="rId2"/>
+    <sheet name="NB Ver 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tree Ver 1" sheetId="4" r:id="rId4"/>
+    <sheet name="SVM Ver 1" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="45">
   <si>
     <t>Features List:</t>
   </si>
@@ -153,15 +154,31 @@
   </si>
   <si>
     <t>Version 3.01</t>
+  </si>
+  <si>
+    <t>min_sample_split</t>
+  </si>
+  <si>
+    <t>Version 1.15</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>kernal</t>
+  </si>
+  <si>
+    <t>rbf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -260,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -270,6 +287,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -584,10 +602,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC652A4-CDC7-409D-B263-D050EE7FDF3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -1534,7 +1552,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{851FA000-8A36-485D-A8EB-9BE4BA802304}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1874,10 +1892,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05CB39-CB07-4783-AABF-8FE9D3C51202}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2202,4 +2220,2044 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J129"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E122" sqref="E122"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="10" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0.83720930232599999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.79069767441899996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.16666666599999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.79069767441899996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.16666666599999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0.81395348837199999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.28571428571399998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="4">
+        <v>0.62068965517200003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="4">
+        <v>0.82352941176500005</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0.77500000000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="4">
+        <v>0.72413793103400004</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" s="4">
+        <v>0.63157894736800002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="3">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73" s="3">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" s="4">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80" s="3">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" t="s">
+        <v>5</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" s="4">
+        <v>0.78947368421099995</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>11</v>
+      </c>
+      <c r="B89" s="3">
+        <v>0.16666700000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H93" t="s">
+        <v>7</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>9</v>
+      </c>
+      <c r="B95" s="4">
+        <v>0.739130434783</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>11</v>
+      </c>
+      <c r="B97" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I101" t="s">
+        <v>14</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>9</v>
+      </c>
+      <c r="B103" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>11</v>
+      </c>
+      <c r="B105" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J109" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111" s="4">
+        <v>0.79166667000000002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>10</v>
+      </c>
+      <c r="B112" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>11</v>
+      </c>
+      <c r="B113" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F117" t="s">
+        <v>5</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H117" t="s">
+        <v>7</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>9</v>
+      </c>
+      <c r="B119" s="4">
+        <v>0.79487179487199999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>10</v>
+      </c>
+      <c r="B120" s="3">
+        <v>0.33333000000000002</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>11</v>
+      </c>
+      <c r="B121" s="3">
+        <v>0.14285700000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>0</v>
+      </c>
+      <c r="B125" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F125" t="s">
+        <v>5</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J125" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>9</v>
+      </c>
+      <c r="B127" s="4">
+        <v>0.71794871794899995</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>10</v>
+      </c>
+      <c r="B128" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>11</v>
+      </c>
+      <c r="B129" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J129"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="10" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.88372093023300002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.88372093023300002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.88372093023300002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0.88372093023300002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="4">
+        <v>0.75862068965499996</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="4">
+        <v>0.88235294117600005</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="4">
+        <v>0.75862068965499996</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" s="4">
+        <v>0.78947368421099995</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" s="4">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" t="s">
+        <v>5</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" s="4">
+        <v>0.89473684210500004</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>11</v>
+      </c>
+      <c r="B89" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H93" t="s">
+        <v>7</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>9</v>
+      </c>
+      <c r="B95" s="4">
+        <v>0.82608695652200004</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>11</v>
+      </c>
+      <c r="B97" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I101" t="s">
+        <v>14</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>9</v>
+      </c>
+      <c r="B103" s="4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>11</v>
+      </c>
+      <c r="B105" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J109" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111" s="4">
+        <v>0.83333333333000004</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>10</v>
+      </c>
+      <c r="B112" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>11</v>
+      </c>
+      <c r="B113" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F117" t="s">
+        <v>5</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H117" t="s">
+        <v>7</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>9</v>
+      </c>
+      <c r="B119" s="4">
+        <v>0.92307692307699996</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>10</v>
+      </c>
+      <c r="B120" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>11</v>
+      </c>
+      <c r="B121" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>0</v>
+      </c>
+      <c r="B125" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F125" t="s">
+        <v>5</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J125" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>9</v>
+      </c>
+      <c r="B127" s="4">
+        <v>0.92307692307699996</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>10</v>
+      </c>
+      <c r="B128" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>11</v>
+      </c>
+      <c r="B129" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>